<commit_message>
2007 Monthly Time Chart Drug Arrests edit
</commit_message>
<xml_diff>
--- a/2007/vi-arrest-data-drug-arrests-2007.xlsx
+++ b/2007/vi-arrest-data-drug-arrests-2007.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet sheetId="1" name="drug-arrests-by-age-and-type-of" state="visible" r:id="rId3"/>
+    <sheet sheetId="2" name="monthly-time-chart" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,6 +17,9 @@
     <t>Drug Type</t>
   </si>
   <si>
+    <t>Month</t>
+  </si>
+  <si>
     <t>Under 10</t>
   </si>
   <si>
@@ -25,6 +29,12 @@
     <t>13--14</t>
   </si>
   <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
     <t>25 29</t>
   </si>
   <si>
@@ -56,6 +66,39 @@
   </si>
   <si>
     <t>“Crack” Cocaine </t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Number of Drug Arrests</t>
   </si>
   <si>
     <t>Cocaine </t>
@@ -172,11 +215,125 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" customWidth="1" max="1" width="35.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>1</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>20</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>22</v>
+      </c>
+      <c t="s" s="1" r="I1">
+        <v>23</v>
+      </c>
+      <c t="s" s="1" r="J1">
+        <v>24</v>
+      </c>
+      <c t="s" s="1" r="K1">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="L1">
+        <v>26</v>
+      </c>
+      <c t="s" s="1" r="M1">
+        <v>27</v>
+      </c>
+      <c s="1" r="N1"/>
+      <c s="1" r="O1"/>
+      <c s="1" r="P1"/>
+      <c s="1" r="Q1"/>
+      <c s="1" r="R1"/>
+      <c s="1" r="S1"/>
+      <c s="1" r="T1"/>
+      <c s="1" r="U1"/>
+      <c s="1" r="V1"/>
+      <c s="1" r="W1"/>
+      <c s="1" r="X1"/>
+      <c s="1" r="Y1"/>
+      <c s="1" r="Z1"/>
+    </row>
+    <row r="2">
+      <c t="s" s="4" r="A2">
+        <v>28</v>
+      </c>
+      <c s="4" r="B2">
+        <v>3059.0</v>
+      </c>
+      <c s="4" r="C2">
+        <v>2742.0</v>
+      </c>
+      <c s="4" r="D2">
+        <v>3370.0</v>
+      </c>
+      <c s="4" r="E2">
+        <v>3098.0</v>
+      </c>
+      <c s="4" r="F2">
+        <v>3113.0</v>
+      </c>
+      <c s="4" r="G2">
+        <v>3053.0</v>
+      </c>
+      <c s="4" r="H2">
+        <v>2913.0</v>
+      </c>
+      <c s="4" r="I2">
+        <v>3057.0</v>
+      </c>
+      <c s="4" r="J2">
+        <v>2903.0</v>
+      </c>
+      <c s="4" r="K2">
+        <v>2989.0</v>
+      </c>
+      <c s="4" r="L2">
+        <v>2711.0</v>
+      </c>
+      <c s="4" r="M2">
+        <v>2512.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -212,13 +369,13 @@
         <v>0</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" s="1" r="C1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c t="s" s="2" r="D1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c s="3" r="E1">
         <v>15.0</v>
@@ -251,41 +408,41 @@
         <v>24.0</v>
       </c>
       <c t="s" s="1" r="O1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c t="s" s="1" r="P1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c t="s" s="1" r="Q1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c t="s" s="1" r="R1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c t="s" s="1" r="S1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c t="s" s="1" r="T1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c t="s" s="1" r="U1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c t="s" s="1" r="V1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c t="s" s="1" r="W1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c t="s" s="1" r="X1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c s="1" r="Y1"/>
       <c s="1" r="Z1"/>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c s="4" r="B2">
         <v>0.0</v>
@@ -359,7 +516,7 @@
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c s="4" r="B3">
         <v>0.0</v>
@@ -433,7 +590,7 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c s="4" r="B4">
         <v>0.0</v>
@@ -507,7 +664,7 @@
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c s="4" r="B5">
         <v>0.0</v>
@@ -581,7 +738,7 @@
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c s="4" r="B6">
         <v>5.0</v>
@@ -655,7 +812,7 @@
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c s="4" r="B7">
         <v>0.0</v>
@@ -731,7 +888,7 @@
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c s="4" r="B8">
         <v>0.0</v>
@@ -805,7 +962,7 @@
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c s="4" r="B9">
         <v>0.0</v>
@@ -879,7 +1036,7 @@
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c s="4" r="B10">
         <v>0.0</v>
@@ -953,7 +1110,7 @@
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c s="4" r="B11">
         <v>0.0</v>
@@ -1027,7 +1184,7 @@
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c s="4" r="B12">
         <v>0.0</v>
@@ -1101,7 +1258,7 @@
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c s="4" r="B13">
         <v>0.0</v>
@@ -1175,7 +1332,7 @@
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c s="4" r="B14">
         <v>0.0</v>
@@ -1250,7 +1407,7 @@
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c s="4" r="B15">
         <v>0.0</v>
@@ -1324,7 +1481,7 @@
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c s="4" r="B16">
         <v>0.0</v>
@@ -1399,7 +1556,7 @@
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c s="4" r="B17">
         <v>0.0</v>
@@ -1473,7 +1630,7 @@
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c s="4" r="B18">
         <v>0.0</v>
@@ -1547,7 +1704,7 @@
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c s="4" r="B19">
         <v>5.0</v>

</xml_diff>